<commit_message>
Updating 0.5 inch aluminum rod to have thicker wall diameter in the parts lists
</commit_message>
<xml_diff>
--- a/Mechanical/Mechanical Integration/Mechanical Integration Parts List.xlsx
+++ b/Mechanical/Mechanical Integration/Mechanical Integration Parts List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\open_source_rover\Documentation\Mechanical Assembly\Final Integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\osr\Mechanical\Mechanical Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,12 +59,6 @@
     <t>0.5”D Collar Clamp</t>
   </si>
   <si>
-    <t>https://www.mcmaster.com/#9056K66</t>
-  </si>
-  <si>
-    <t>7237K59</t>
-  </si>
-  <si>
     <t>S16</t>
   </si>
   <si>
@@ -117,6 +111,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>89965K364</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#89965K364</t>
   </si>
 </sst>
 </file>
@@ -126,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -147,6 +147,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,10 +222,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -228,21 +243,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,203 +561,202 @@
   <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.1328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="36.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15">
+        <v>100</v>
+      </c>
+      <c r="C2" s="15">
         <v>20</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="D2" s="16">
         <v>100</v>
       </c>
-      <c r="C2" s="8">
-        <v>20</v>
-      </c>
-      <c r="D2" s="9">
-        <v>100</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="8" t="s">
+      <c r="F2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="18">
         <v>4.49</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="18">
         <f>B2/D2*I2</f>
         <v>4.49</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>14</v>
+      <c r="K2" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="8">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="11">
         <v>1</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="12">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="10">
-        <v>22.57</v>
-      </c>
-      <c r="J3" s="10">
-        <f>B3/D3*I3</f>
-        <v>22.57</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>10</v>
+      <c r="I3" s="19">
+        <v>23.16</v>
+      </c>
+      <c r="J3" s="19">
+        <v>23.16</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="15">
         <v>6</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="15">
         <v>6</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="18">
         <v>2.2599999999999998</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="18">
         <f>B4/D4*I4</f>
         <v>13.559999999999999</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="15">
         <v>8</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="15">
         <v>8</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="16">
         <v>2</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="17">
         <v>545532</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="18">
         <v>3.99</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="18">
         <f>B5/D5*I5</f>
         <v>15.96</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L5" s="2"/>
@@ -728,13 +764,13 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J8" s="12">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="J8" s="9">
         <f>SUM(J2:J5)</f>
-        <v>56.580000000000005</v>
+        <v>57.169999999999995</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -744,9 +780,8 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" location="9056K66"/>
-    <hyperlink ref="K4" r:id="rId2" location="368=229"/>
-    <hyperlink ref="K5" r:id="rId3"/>
+    <hyperlink ref="K4" r:id="rId1" location="368=229"/>
+    <hyperlink ref="K5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>